<commit_message>
fixed the reports, hopefully for the last time
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>input3</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>input2</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
@@ -169,11 +166,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="705809209"/>
-        <c:axId val="1084284550"/>
+        <c:axId val="680425450"/>
+        <c:axId val="641079840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="705809209"/>
+        <c:axId val="680425450"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -188,10 +185,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1084284550"/>
+        <c:crossAx val="641079840"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1084284550"/>
+        <c:axId val="641079840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -239,7 +236,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705809209"/>
+        <c:crossAx val="680425450"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -298,11 +295,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="146134957"/>
-        <c:axId val="1447467889"/>
+        <c:axId val="1156609998"/>
+        <c:axId val="1657444588"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="146134957"/>
+        <c:axId val="1156609998"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -317,10 +314,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1447467889"/>
+        <c:crossAx val="1657444588"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1447467889"/>
+        <c:axId val="1657444588"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +365,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="146134957"/>
+        <c:crossAx val="1156609998"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -427,11 +424,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1557873276"/>
-        <c:axId val="969667279"/>
+        <c:axId val="651737587"/>
+        <c:axId val="557552807"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1557873276"/>
+        <c:axId val="651737587"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -446,10 +443,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="969667279"/>
+        <c:crossAx val="557552807"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="969667279"/>
+        <c:axId val="557552807"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -497,7 +494,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1557873276"/>
+        <c:crossAx val="651737587"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -556,11 +553,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1625578699"/>
-        <c:axId val="1673206627"/>
+        <c:axId val="1353888183"/>
+        <c:axId val="1291265517"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1625578699"/>
+        <c:axId val="1353888183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -575,10 +572,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1673206627"/>
+        <c:crossAx val="1291265517"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1673206627"/>
+        <c:axId val="1291265517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -626,7 +623,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1625578699"/>
+        <c:crossAx val="1353888183"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -685,11 +682,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="985763580"/>
-        <c:axId val="1502894961"/>
+        <c:axId val="1269145729"/>
+        <c:axId val="1528226338"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="985763580"/>
+        <c:axId val="1269145729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -704,10 +701,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1502894961"/>
+        <c:crossAx val="1528226338"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1502894961"/>
+        <c:axId val="1528226338"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +752,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="985763580"/>
+        <c:crossAx val="1269145729"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -814,11 +811,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1733876633"/>
-        <c:axId val="2141503469"/>
+        <c:axId val="527831642"/>
+        <c:axId val="1990098048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1733876633"/>
+        <c:axId val="527831642"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,10 +830,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2141503469"/>
+        <c:crossAx val="1990098048"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141503469"/>
+        <c:axId val="1990098048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +881,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1733876633"/>
+        <c:crossAx val="527831642"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -943,11 +940,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1486744181"/>
-        <c:axId val="135861688"/>
+        <c:axId val="976865397"/>
+        <c:axId val="488984290"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1486744181"/>
+        <c:axId val="976865397"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -962,10 +959,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="135861688"/>
+        <c:crossAx val="488984290"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="135861688"/>
+        <c:axId val="488984290"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,7 +1010,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1486744181"/>
+        <c:crossAx val="976865397"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1048,6 +1045,7 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1072,11 +1070,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="343092921"/>
-        <c:axId val="1199672354"/>
+        <c:overlap val="100"/>
+        <c:axId val="544573712"/>
+        <c:axId val="299237292"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="343092921"/>
+        <c:axId val="544573712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1091,10 +1090,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1199672354"/>
+        <c:crossAx val="299237292"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1199672354"/>
+        <c:axId val="299237292"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1142,7 +1141,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="343092921"/>
+        <c:crossAx val="544573712"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1201,11 +1200,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1848190485"/>
-        <c:axId val="202012394"/>
+        <c:axId val="713907528"/>
+        <c:axId val="792813569"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1848190485"/>
+        <c:axId val="713907528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1220,10 +1219,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202012394"/>
+        <c:crossAx val="792813569"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="202012394"/>
+        <c:axId val="792813569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,7 +1270,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848190485"/>
+        <c:crossAx val="713907528"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1330,11 +1329,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="834860533"/>
-        <c:axId val="869987498"/>
+        <c:axId val="1504270179"/>
+        <c:axId val="1792426200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="834860533"/>
+        <c:axId val="1504270179"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1349,10 +1348,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="869987498"/>
+        <c:crossAx val="1792426200"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="869987498"/>
+        <c:axId val="1792426200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1399,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="834860533"/>
+        <c:crossAx val="1504270179"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1485,11 +1484,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1532495900"/>
-        <c:axId val="598845218"/>
+        <c:axId val="1509789183"/>
+        <c:axId val="2003981700"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1532495900"/>
+        <c:axId val="1509789183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1506,10 +1505,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="598845218"/>
+        <c:crossAx val="2003981700"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="598845218"/>
+        <c:axId val="2003981700"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1561,7 +1560,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1532495900"/>
+        <c:crossAx val="1509789183"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1631,11 +1630,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1824571613"/>
-        <c:axId val="1580081642"/>
+        <c:axId val="709178773"/>
+        <c:axId val="155581264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1824571613"/>
+        <c:axId val="709178773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1650,10 +1649,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1580081642"/>
+        <c:crossAx val="155581264"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1580081642"/>
+        <c:axId val="155581264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1701,7 +1700,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1824571613"/>
+        <c:crossAx val="709178773"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1760,11 +1759,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="361950218"/>
-        <c:axId val="728560527"/>
+        <c:axId val="1956556750"/>
+        <c:axId val="1674443195"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="361950218"/>
+        <c:axId val="1956556750"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1779,10 +1778,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="728560527"/>
+        <c:crossAx val="1674443195"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="728560527"/>
+        <c:axId val="1674443195"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1829,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="361950218"/>
+        <c:crossAx val="1956556750"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1889,11 +1888,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="196583298"/>
-        <c:axId val="521410524"/>
+        <c:axId val="673289305"/>
+        <c:axId val="441188424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="196583298"/>
+        <c:axId val="673289305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1908,10 +1907,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="521410524"/>
+        <c:crossAx val="441188424"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="521410524"/>
+        <c:axId val="441188424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +1958,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="196583298"/>
+        <c:crossAx val="673289305"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2018,11 +2017,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="1563546809"/>
-        <c:axId val="36032293"/>
+        <c:axId val="1827179378"/>
+        <c:axId val="547096517"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1563546809"/>
+        <c:axId val="1827179378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,10 +2036,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36032293"/>
+        <c:crossAx val="547096517"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36032293"/>
+        <c:axId val="547096517"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2088,7 +2087,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1563546809"/>
+        <c:crossAx val="1827179378"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2111,7 +2110,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvPr id="1" name="Chart 2" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2136,7 +2135,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2161,7 +2160,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2241,7 +2240,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name="Chart 1" title="Gráfico"/>
+        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2266,7 +2265,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
+        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2291,7 +2290,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2316,7 +2315,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 8" title="Gráfico"/>
+        <xdr:cNvPr id="10" name="Chart 10" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2341,7 +2340,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name="Chart 11" title="Gráfico"/>
+        <xdr:cNvPr id="12" name="Chart 12" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2396,7 +2395,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2421,7 +2420,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Gráfico"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2446,7 +2445,7 @@
     <xdr:ext cx="5715000" cy="3533775"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 10" title="Gráfico"/>
+        <xdr:cNvPr id="11" name="Chart 11" title="Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2546,8 +2545,8 @@
       <c r="C3" s="5">
         <v>12.0</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>14</v>
+      <c r="D3" s="6">
+        <v>0.0</v>
       </c>
       <c r="E3" s="5">
         <v>20.0</v>
@@ -2572,8 +2571,8 @@
       <c r="C4" s="3">
         <v>0.098</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
+      <c r="D4" s="7">
+        <v>0.0</v>
       </c>
       <c r="E4" s="3">
         <v>7.15</v>
@@ -2585,7 +2584,7 @@
         <v>0.562</v>
       </c>
       <c r="H4" s="3">
-        <v>52.745</v>
+        <v>1.263</v>
       </c>
     </row>
     <row r="5">
@@ -2598,8 +2597,8 @@
       <c r="C5" s="5">
         <v>6746.0</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
+      <c r="D5" s="6">
+        <v>0.0</v>
       </c>
       <c r="E5" s="5">
         <v>745852.0</v>
@@ -2611,7 +2610,7 @@
         <v>29513.0</v>
       </c>
       <c r="H5" s="5">
-        <v>627274.0</v>
+        <v>12084.0</v>
       </c>
     </row>
     <row r="6">
@@ -2624,8 +2623,8 @@
       <c r="C6" s="5">
         <v>23500.0</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>14</v>
+      <c r="D6" s="6">
+        <v>0.0</v>
       </c>
       <c r="E6" s="5">
         <v>52.0</v>
@@ -2650,8 +2649,8 @@
       <c r="C7" s="5">
         <v>34382.0</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
+      <c r="D7" s="6">
+        <v>0.0</v>
       </c>
       <c r="E7" s="5">
         <v>3470238.0</v>
@@ -2663,7 +2662,7 @@
         <v>107476.0</v>
       </c>
       <c r="H7" s="5">
-        <v>2840192.0</v>
+        <v>57667.0</v>
       </c>
     </row>
     <row r="8">
@@ -2758,7 +2757,7 @@
         <v>0.012</v>
       </c>
       <c r="H4" s="1">
-        <v>0.03</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="5">
@@ -2784,7 +2783,7 @@
         <v>37.0</v>
       </c>
       <c r="H5" s="1">
-        <v>574.0</v>
+        <v>298.0</v>
       </c>
     </row>
     <row r="6">
@@ -2836,7 +2835,7 @@
         <v>145.0</v>
       </c>
       <c r="H7" s="1">
-        <v>2855.0</v>
+        <v>1523.0</v>
       </c>
     </row>
     <row r="13">
@@ -2933,8 +2932,8 @@
       <c r="G4" s="1">
         <v>0.594</v>
       </c>
-      <c r="H4" s="1">
-        <v>125.04</v>
+      <c r="H4" s="2">
+        <v>0.788</v>
       </c>
     </row>
     <row r="5">
@@ -2960,7 +2959,7 @@
         <v>46921.0</v>
       </c>
       <c r="H5" s="1">
-        <v>2.7118392E7</v>
+        <v>37657.0</v>
       </c>
     </row>
     <row r="6">
@@ -3012,7 +3011,7 @@
         <v>175899.0</v>
       </c>
       <c r="H7" s="1">
-        <v>9.8050126E7</v>
+        <v>148996.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>